<commit_message>
Add pulse generators for RST_EXT pads, and clock enables for replenishment clocks. Update simulation, scripts, reg map.
</commit_message>
<xml_diff>
--- a/doc/qpix_fw_reg_map.xlsx
+++ b/doc/qpix_fw_reg_map.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="117">
   <si>
     <t>reg num</t>
   </si>
@@ -66,9 +66,6 @@
     <t>43c00000</t>
   </si>
   <si>
-    <t>control</t>
-  </si>
-  <si>
     <t>data1</t>
   </si>
   <si>
@@ -111,12 +108,6 @@
     <t>5'b0, xmit1, load1, rst1</t>
   </si>
   <si>
-    <t>6'b0, opad2_control, opad_control</t>
-  </si>
-  <si>
-    <t>6'b0, opad2_cal_control, opad_cal_control</t>
-  </si>
-  <si>
     <t>6'b0, opad2_startup, opad_startup</t>
   </si>
   <si>
@@ -142,9 +133,6 @@
   </si>
   <si>
     <t>FIFO read control</t>
-  </si>
-  <si>
-    <t>4'b0, 2_RST_EXT, RST_EXT,  Ext_POR, sys_rst</t>
   </si>
   <si>
     <t>trig ts [63:56]</t>
@@ -399,6 +387,21 @@
   </si>
   <si>
     <t>6'b0, opad2_selDefData, loadData2</t>
+  </si>
+  <si>
+    <t>4'b0, pulse_rst_ext2, pulse_rst_ext,  Ext_POR, sys_rst</t>
+  </si>
+  <si>
+    <t>4'b0, opad2_cal_control, opad_cal_control, pad2_control, opad_control</t>
+  </si>
+  <si>
+    <t>6'b0, clk2_repl_en, clk_repl_en</t>
+  </si>
+  <si>
+    <t>control (pulse, level, gating)</t>
+  </si>
+  <si>
+    <t>control2 (programmable pulse)</t>
   </si>
 </sst>
 </file>
@@ -847,7 +850,7 @@
   <dimension ref="A1:I68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -856,10 +859,10 @@
     <col min="2" max="2" width="9.6640625" customWidth="1"/>
     <col min="3" max="3" width="11.5546875" customWidth="1"/>
     <col min="4" max="4" width="30.88671875" customWidth="1"/>
-    <col min="5" max="5" width="36.88671875" customWidth="1"/>
-    <col min="6" max="6" width="30.33203125" customWidth="1"/>
-    <col min="7" max="7" width="37.77734375" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="26.6640625" customWidth="1"/>
+    <col min="6" max="6" width="60.21875" customWidth="1"/>
+    <col min="7" max="7" width="44.6640625" customWidth="1"/>
+    <col min="8" max="8" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -901,7 +904,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>0</v>
       </c>
@@ -913,19 +916,19 @@
         <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>29</v>
+        <v>114</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>28</v>
+        <v>113</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>39</v>
+        <v>112</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I5" s="2"/>
     </row>
@@ -948,13 +951,13 @@
         <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I6" s="2"/>
     </row>
@@ -971,19 +974,19 @@
         <v>9</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="H7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I7" s="2"/>
     </row>
@@ -1006,13 +1009,13 @@
         <v>10</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I8" s="2"/>
     </row>
@@ -1029,19 +1032,19 @@
         <v>9</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="H9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I9" s="2"/>
     </row>
@@ -1067,10 +1070,10 @@
         <v>10</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I10" s="2"/>
     </row>
@@ -1093,13 +1096,13 @@
         <v>10</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I11" s="2"/>
     </row>
@@ -1112,12 +1115,16 @@
         <f t="shared" si="0"/>
         <v>43C0001C</v>
       </c>
-      <c r="C12" s="7"/>
+      <c r="C12" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="H12" s="7" t="s">
+        <v>116</v>
+      </c>
       <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -2115,7 +2122,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1</v>
@@ -2151,29 +2158,29 @@
         <v>0</v>
       </c>
       <c r="C5" s="2" t="str">
-        <f>DEC2HEX(HEX2DEC($A$2)+(A5)*4)</f>
+        <f t="shared" ref="C5:C20" si="0">DEC2HEX(HEX2DEC($A$2)+(A5)*4)</f>
         <v>43C00100</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -2182,1102 +2189,1102 @@
         <v>65</v>
       </c>
       <c r="B6" s="10">
-        <f t="shared" ref="B6:B68" si="0">A6-64</f>
+        <f t="shared" ref="B6:B68" si="1">A6-64</f>
         <v>1</v>
       </c>
       <c r="C6" s="2" t="str">
-        <f>DEC2HEX(HEX2DEC($A$2)+(A6)*4)</f>
+        <f t="shared" si="0"/>
         <v>43C00104</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <f t="shared" ref="A7:A68" si="1">A6+1</f>
+        <f t="shared" ref="A7:A68" si="2">A6+1</f>
         <v>66</v>
       </c>
       <c r="B7" s="10">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="C7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C7" s="6" t="str">
-        <f>DEC2HEX(HEX2DEC($A$2)+(A7)*4)</f>
         <v>43C00108</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>67</v>
       </c>
       <c r="B8" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="C8" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C8" s="6" t="str">
-        <f>DEC2HEX(HEX2DEC($A$2)+(A8)*4)</f>
         <v>43C0010C</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>68</v>
       </c>
       <c r="B9" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="C9" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C9" s="2" t="str">
-        <f>DEC2HEX(HEX2DEC($A$2)+(A9)*4)</f>
         <v>43C00110</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>69</v>
       </c>
       <c r="B10" s="10">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C10" s="2" t="str">
-        <f>DEC2HEX(HEX2DEC($A$2)+(A10)*4)</f>
         <v>43C00114</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
       <c r="B11" s="10">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C11" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C11" s="2" t="str">
-        <f>DEC2HEX(HEX2DEC($A$2)+(A11)*4)</f>
         <v>43C00118</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>71</v>
       </c>
       <c r="B12" s="10">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C12" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C12" s="2" t="str">
-        <f>DEC2HEX(HEX2DEC($A$2)+(A12)*4)</f>
         <v>43C0011C</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>72</v>
       </c>
       <c r="B13" s="10">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="C13" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C13" s="2" t="str">
-        <f>DEC2HEX(HEX2DEC($A$2)+(A13)*4)</f>
         <v>43C00120</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>73</v>
       </c>
       <c r="B14" s="10">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="C14" s="2" t="str">
-        <f>DEC2HEX(HEX2DEC($A$2)+(A14)*4)</f>
         <v>43C00124</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>74</v>
       </c>
       <c r="B15" s="10">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="C15" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C15" s="2" t="str">
-        <f>DEC2HEX(HEX2DEC($A$2)+(A15)*4)</f>
         <v>43C00128</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
       <c r="B16" s="10">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="C16" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="C16" s="2" t="str">
-        <f>DEC2HEX(HEX2DEC($A$2)+(A16)*4)</f>
         <v>43C0012C</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>76</v>
       </c>
       <c r="B17" s="10">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="C17" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="C17" s="2" t="str">
-        <f>DEC2HEX(HEX2DEC($A$2)+(A17)*4)</f>
         <v>43C00130</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>77</v>
       </c>
       <c r="B18" s="10">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="C18" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="C18" s="2" t="str">
-        <f>DEC2HEX(HEX2DEC($A$2)+(A18)*4)</f>
         <v>43C00134</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="J18" s="2"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>78</v>
       </c>
       <c r="B19" s="10">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="C19" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="C19" s="2" t="str">
-        <f>DEC2HEX(HEX2DEC($A$2)+(A19)*4)</f>
         <v>43C00138</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>79</v>
       </c>
       <c r="B20" s="10">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="C20" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="C20" s="2" t="str">
-        <f>DEC2HEX(HEX2DEC($A$2)+(A20)*4)</f>
         <v>43C0013C</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="B21" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="C21" s="2" t="str">
-        <f t="shared" ref="C21:C68" si="2">DEC2HEX(HEX2DEC($A$2)+(A21)*4)</f>
+        <f t="shared" ref="C21:C68" si="3">DEC2HEX(HEX2DEC($A$2)+(A21)*4)</f>
         <v>43C00140</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
       <c r="B22" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="C22" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C00144</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>82</v>
       </c>
       <c r="B23" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="C23" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C00148</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J23" s="2"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>83</v>
       </c>
       <c r="B24" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="C24" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C0014C</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="J24" s="2"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>84</v>
       </c>
       <c r="B25" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C25" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C00150</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="J25" s="2"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>85</v>
       </c>
       <c r="B26" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="C26" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C00154</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>86</v>
       </c>
       <c r="B27" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="C27" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C00158</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>87</v>
       </c>
       <c r="B28" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="C28" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C0015C</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>88</v>
       </c>
       <c r="B29" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="C29" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C00160</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="J29" s="2"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>89</v>
       </c>
       <c r="B30" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="C30" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C00164</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="J30" s="2"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>90</v>
       </c>
       <c r="B31" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="C31" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C00168</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="J31" s="2"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>91</v>
       </c>
       <c r="B32" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="C32" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C0016C</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="J32" s="2"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>92</v>
       </c>
       <c r="B33" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="C33" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C00170</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="J33" s="2"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>93</v>
       </c>
       <c r="B34" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="C34" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C00174</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="J34" s="2"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>94</v>
       </c>
       <c r="B35" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="C35" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C00178</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J35" s="2"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>95</v>
       </c>
       <c r="B36" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="C36" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C0017C</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="J36" s="2"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>96</v>
       </c>
       <c r="B37" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="C37" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C00180</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="J37" s="2"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>97</v>
       </c>
       <c r="B38" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="C38" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C00184</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="J38" s="2"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>98</v>
       </c>
       <c r="B39" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="C39" s="14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C00188</v>
       </c>
       <c r="D39" s="7"/>
@@ -3290,15 +3297,15 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>99</v>
       </c>
       <c r="B40" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="C40" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C0018C</v>
       </c>
       <c r="D40" s="7"/>
@@ -3311,15 +3318,15 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="B41" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="C41" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C00190</v>
       </c>
       <c r="D41" s="7"/>
@@ -3332,15 +3339,15 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>101</v>
       </c>
       <c r="B42" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="C42" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C00194</v>
       </c>
       <c r="D42" s="7"/>
@@ -3353,15 +3360,15 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>102</v>
       </c>
       <c r="B43" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="C43" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C00198</v>
       </c>
       <c r="D43" s="7"/>
@@ -3374,15 +3381,15 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>103</v>
       </c>
       <c r="B44" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="C44" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C0019C</v>
       </c>
       <c r="D44" s="7"/>
@@ -3395,15 +3402,15 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>104</v>
       </c>
       <c r="B45" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="C45" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C001A0</v>
       </c>
       <c r="D45" s="7"/>
@@ -3416,15 +3423,15 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>105</v>
       </c>
       <c r="B46" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="C46" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C001A4</v>
       </c>
       <c r="D46" s="7"/>
@@ -3437,15 +3444,15 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>106</v>
       </c>
       <c r="B47" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="C47" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C001A8</v>
       </c>
       <c r="D47" s="7"/>
@@ -3458,15 +3465,15 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>107</v>
       </c>
       <c r="B48" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="C48" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C001AC</v>
       </c>
       <c r="D48" s="7"/>
@@ -3479,15 +3486,15 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>108</v>
       </c>
       <c r="B49" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="C49" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C001B0</v>
       </c>
       <c r="D49" s="7"/>
@@ -3500,15 +3507,15 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>109</v>
       </c>
       <c r="B50" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="C50" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C001B4</v>
       </c>
       <c r="D50" s="2" t="s">
@@ -3521,27 +3528,27 @@
         <v>10</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="J50" s="2"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>110</v>
       </c>
       <c r="B51" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="C51" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C001B8</v>
       </c>
       <c r="D51" s="2" t="s">
@@ -3554,27 +3561,27 @@
         <v>10</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="J51" s="2"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>111</v>
       </c>
       <c r="B52" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="C52" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C001BC</v>
       </c>
       <c r="D52" s="2" t="s">
@@ -3587,27 +3594,27 @@
         <v>10</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="J52" s="2"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>112</v>
       </c>
       <c r="B53" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="C53" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C001C0</v>
       </c>
       <c r="D53" s="2" t="s">
@@ -3620,27 +3627,27 @@
         <v>10</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H53" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I53" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="I53" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="J53" s="2"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>113</v>
       </c>
       <c r="B54" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="C54" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C001C4</v>
       </c>
       <c r="D54" s="2" t="s">
@@ -3653,27 +3660,27 @@
         <v>10</v>
       </c>
       <c r="G54" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I54" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I54" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="J54" s="2"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>114</v>
       </c>
       <c r="B55" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="C55" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C001C8</v>
       </c>
       <c r="D55" s="2" t="s">
@@ -3686,27 +3693,27 @@
         <v>10</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J55" s="2"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>115</v>
       </c>
       <c r="B56" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="C56" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C001CC</v>
       </c>
       <c r="D56" s="2" t="s">
@@ -3719,27 +3726,27 @@
         <v>10</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J56" s="2"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>116</v>
       </c>
       <c r="B57" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="C57" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C001D0</v>
       </c>
       <c r="D57" s="2" t="s">
@@ -3752,27 +3759,27 @@
         <v>10</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J57" s="2"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>117</v>
       </c>
       <c r="B58" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="C58" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C001D4</v>
       </c>
       <c r="D58" s="2" t="s">
@@ -3785,27 +3792,27 @@
         <v>10</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="J58" s="2"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>118</v>
       </c>
       <c r="B59" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="C59" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C001D8</v>
       </c>
       <c r="D59" s="2" t="s">
@@ -3818,27 +3825,27 @@
         <v>10</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="J59" s="2"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>119</v>
       </c>
       <c r="B60" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="C60" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C001DC</v>
       </c>
       <c r="D60" s="2" t="s">
@@ -3851,27 +3858,27 @@
         <v>10</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="J60" s="2"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>120</v>
       </c>
       <c r="B61" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>56</v>
       </c>
       <c r="C61" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C001E0</v>
       </c>
       <c r="D61" s="2" t="s">
@@ -3884,27 +3891,27 @@
         <v>10</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J61" s="2"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>121</v>
       </c>
       <c r="B62" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="C62" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C001E4</v>
       </c>
       <c r="D62" s="2" t="s">
@@ -3917,27 +3924,27 @@
         <v>10</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="J62" s="2"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>122</v>
       </c>
       <c r="B63" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="C63" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C001E8</v>
       </c>
       <c r="D63" s="2" t="s">
@@ -3950,27 +3957,27 @@
         <v>10</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="J63" s="2"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>123</v>
       </c>
       <c r="B64" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>59</v>
       </c>
       <c r="C64" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C001EC</v>
       </c>
       <c r="D64" s="2" t="s">
@@ -3983,27 +3990,27 @@
         <v>10</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="J64" s="2"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>124</v>
       </c>
       <c r="B65" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="C65" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C001F0</v>
       </c>
       <c r="D65" s="2" t="s">
@@ -4016,27 +4023,27 @@
         <v>10</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J65" s="2"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>125</v>
       </c>
       <c r="B66" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>61</v>
       </c>
       <c r="C66" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C001F4</v>
       </c>
       <c r="D66" s="7"/>
@@ -4049,15 +4056,15 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>126</v>
       </c>
       <c r="B67" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>62</v>
       </c>
       <c r="C67" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C001F8</v>
       </c>
       <c r="D67" s="7"/>
@@ -4070,34 +4077,34 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>127</v>
       </c>
       <c r="B68" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63</v>
       </c>
       <c r="C68" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43C001FC</v>
       </c>
       <c r="D68" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E68" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F68" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G68" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H68" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="E68" s="8" t="s">
+      <c r="I68" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="F68" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="G68" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="H68" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="I68" s="8" t="s">
-        <v>57</v>
       </c>
       <c r="J68" s="8"/>
     </row>

</xml_diff>